<commit_message>
Fixed bug; worked on ExcelUX
</commit_message>
<xml_diff>
--- a/tbx/sandbox/BEAR6-EstimationUX.xlsx
+++ b/tbx/sandbox/BEAR6-EstimationUX.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myself/Documents/ogr-external-projects/ecb-bear/BEAR-toolbox/tbx/sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58653FC-1697-F24A-9623-04CDD13C9943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCC26E3-8D6B-3044-B032-4BA25E3E3C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{F4E23125-5A47-B048-90D5-D780F816F882}"/>
   </bookViews>
   <sheets>
     <sheet name="Data source" sheetId="1" r:id="rId1"/>
     <sheet name="Meta information" sheetId="3" r:id="rId2"/>
-    <sheet name="Reduced-form estimator" sheetId="4" r:id="rId3"/>
-    <sheet name="Structural identifier" sheetId="5" r:id="rId4"/>
+    <sheet name="Reduced-form estimation" sheetId="4" r:id="rId3"/>
+    <sheet name="Structural identification" sheetId="5" r:id="rId4"/>
     <sheet name="_Backend" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -229,12 +229,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{061D4620-3678-5E4D-A51F-FC6933FACFF2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter an identification horizon as the number of periods for which the impulse responses and FEVDs will be calculated, including in the structural identification step</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>x</t>
   </si>
@@ -303,6 +327,12 @@
   </si>
   <si>
     <t>Oil</t>
+  </si>
+  <si>
+    <t>1975-Q1</t>
+  </si>
+  <si>
+    <t>2014-Q4</t>
   </si>
 </sst>
 </file>
@@ -806,7 +836,7 @@
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C6A45731-F5FB-4447-B81B-51C96E30823B}">
           <x14:formula1>
             <xm:f>_Backend!$B$2:$B$4</xm:f>
@@ -824,7 +854,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.25"/>
@@ -886,23 +916,25 @@
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="8">
-        <v>1975</v>
+      <c r="B7" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="8">
-        <v>2014</v>
+      <c r="B8" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="7">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">

</xml_diff>